<commit_message>
- Admin Panel Set up - Property Insert opeartion ongoing...
</commit_message>
<xml_diff>
--- a/Documentation/DB_Design.xlsx
+++ b/Documentation/DB_Design.xlsx
@@ -20,9 +20,120 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t xml:space="preserve">Properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testimonials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Star</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GoogleMapLocation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bedroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bathroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balcony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wifi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telephone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jacuzzi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DoubleBed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alarm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gym</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FloorPlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VideoLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IsFeatured</t>
   </si>
 </sst>
 </file>
@@ -32,11 +143,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -53,8 +165,16 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFD7"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -63,8 +183,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFBF0041"/>
+        <bgColor rgb="FF800080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00A933"/>
+        <bgColor rgb="FF008000"/>
       </patternFill>
     </fill>
   </fills>
@@ -102,13 +228,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -120,6 +250,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FFBF0041"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFD7"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF00A933"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -128,17 +318,204 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B4"/>
+  <dimension ref="B4:D39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.55"/>
+  </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>